<commit_message>
net skip threshold modified
</commit_message>
<xml_diff>
--- a/result/record.xlsx
+++ b/result/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Garage\Code\LC-VLSICAD\project\FPGA_r_op\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14609C2F-6E7C-4EB8-AC76-13C3ACDC3750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE87E4C2-B611-4A12-8D31-986714A547BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6831" yWindow="6036" windowWidth="22119" windowHeight="11613" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6831" yWindow="4274" windowWidth="22119" windowHeight="11612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="25.35" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -426,10 +426,22 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>